<commit_message>
initial diagramn for instrument control
</commit_message>
<xml_diff>
--- a/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
+++ b/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="210">
   <si>
     <t>Usage</t>
   </si>
@@ -522,9 +522,6 @@
     <t>Mac OS X Mountain Lion 10.8.4</t>
   </si>
   <si>
-    <t>WinXP system tests</t>
-  </si>
-  <si>
     <t>ndw675</t>
   </si>
   <si>
@@ -663,14 +660,35 @@
     <t>Ubuntu 14.04 64-bit</t>
   </si>
   <si>
-    <t>Interview PC</t>
+    <t>recycled</t>
+  </si>
+  <si>
+    <t>Fedora 20 build Server</t>
+  </si>
+  <si>
+    <t>On order</t>
+  </si>
+  <si>
+    <t>Precision T7810</t>
+  </si>
+  <si>
+    <t>2x Xeon Processor E5-2687W v3 (10C, 3.1GHz, Turbo, HT, 25M, 160W)</t>
+  </si>
+  <si>
+    <t>512GB SSD + 2TB HDD</t>
+  </si>
+  <si>
+    <t>NVIDIA Quadro K620</t>
+  </si>
+  <si>
+    <t>Fedora 20 64-Bit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -689,13 +707,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -707,10 +743,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -720,8 +757,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -838,6 +882,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 3" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 3" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1158,7 +1288,7 @@
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1969,7 +2099,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
         <v>127</v>
@@ -2043,7 +2173,7 @@
     </row>
     <row r="26" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s">
         <v>137</v>
@@ -2152,67 +2282,67 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I29" t="s">
-        <v>163</v>
-      </c>
-      <c r="J29">
+      <c r="J29" s="3">
         <f>VLOOKUP(E29,Benchmarks!$A$2:$B$999,2,FALSE)</f>
         <v>1497</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="3">
         <f>VLOOKUP(H29,Benchmarks!$D$2:$E$999,2,FALSE)</f>
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" t="s">
         <v>164</v>
-      </c>
-      <c r="B30" t="s">
-        <v>165</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
       </c>
       <c r="D30" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" t="s">
         <v>166</v>
-      </c>
-      <c r="E30" t="s">
-        <v>167</v>
       </c>
       <c r="F30" t="s">
         <v>108</v>
       </c>
       <c r="G30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I30" t="s">
         <v>129</v>
@@ -2228,28 +2358,28 @@
     </row>
     <row r="31" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" t="s">
         <v>169</v>
-      </c>
-      <c r="B31" t="s">
-        <v>170</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
       </c>
       <c r="D31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" t="s">
         <v>171</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>172</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>173</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>174</v>
-      </c>
-      <c r="H31" t="s">
-        <v>175</v>
       </c>
       <c r="I31" t="s">
         <v>129</v>
@@ -2265,28 +2395,28 @@
     </row>
     <row r="32" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" t="s">
         <v>176</v>
-      </c>
-      <c r="B32" t="s">
-        <v>177</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="D32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E32" t="s">
         <v>178</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>179</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>180</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>181</v>
-      </c>
-      <c r="H32" t="s">
-        <v>182</v>
       </c>
       <c r="I32" t="s">
         <v>126</v>
@@ -2300,58 +2430,58 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>203</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H33" t="s">
-        <v>162</v>
-      </c>
-      <c r="I33" t="s">
-        <v>202</v>
-      </c>
-      <c r="J33">
+      <c r="H33" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J33" s="3">
         <f>VLOOKUP(E33,Benchmarks!$A$2:$B$999,2,FALSE)</f>
         <v>1964</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="3">
         <f>VLOOKUP(H33,Benchmarks!$D$2:$E$999,2,FALSE)</f>
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B34" t="s">
         <v>198</v>
-      </c>
-      <c r="B34" t="s">
-        <v>199</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>30</v>
@@ -2360,10 +2490,10 @@
         <v>43</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J34">
         <f>VLOOKUP(E34,Benchmarks!$A$2:$B$999,2,FALSE)</f>
@@ -2376,7 +2506,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
         <v>65</v>
@@ -2411,14 +2541,41 @@
         <v>987</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J36" t="e">
+    <row r="36" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>205</v>
+      </c>
+      <c r="E36" t="s">
+        <v>206</v>
+      </c>
+      <c r="F36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" t="s">
+        <v>207</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J36">
         <f>VLOOKUP(E36,Benchmarks!$A$2:$B$999,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K36" t="e">
+        <v>0</v>
+      </c>
+      <c r="K36">
         <f>VLOOKUP(H36,Benchmarks!$D$2:$E$999,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -2433,10 +2590,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>30</v>
@@ -2952,17 +3109,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2972,17 +3130,17 @@
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -3086,7 +3244,7 @@
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8">
         <v>7679</v>
@@ -3246,7 +3404,7 @@
         <v>3927</v>
       </c>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E19">
         <v>11</v>
@@ -3254,13 +3412,13 @@
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B20">
         <v>1497</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E20">
         <v>33</v>
@@ -3268,13 +3426,13 @@
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B21">
         <v>1964</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E21">
         <v>6</v>
@@ -3282,13 +3440,13 @@
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B22">
         <v>405</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E22">
         <v>658</v>
@@ -3296,15 +3454,18 @@
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B23">
         <v>16874</v>
       </c>
+      <c r="D23" s="4" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24">
         <v>19522</v>
@@ -3312,7 +3473,7 @@
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25">
         <v>1546</v>
@@ -3320,10 +3481,15 @@
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B26">
         <v>9447</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update hardware for new servers
</commit_message>
<xml_diff>
--- a/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
+++ b/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="555" windowWidth="21495" windowHeight="13725"/>
+    <workbookView xWindow="525" yWindow="555" windowWidth="21495" windowHeight="13725" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Desktops" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="230">
   <si>
     <t>Usage</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Spare Laptop 1</t>
   </si>
   <si>
-    <t>3GB</t>
-  </si>
-  <si>
     <t>Spare Laptop 2</t>
   </si>
   <si>
@@ -441,21 +438,9 @@
     <t>Intel Q35</t>
   </si>
   <si>
-    <t>Performance tests</t>
-  </si>
-  <si>
-    <t>mantidlnx02</t>
-  </si>
-  <si>
-    <t>OptiPlex GX620</t>
-  </si>
-  <si>
     <t>Pentium 4 CPU 3.40GHz (2 core no HT)</t>
   </si>
   <si>
-    <t>250GB IDE</t>
-  </si>
-  <si>
     <t>Autoreduction server</t>
   </si>
   <si>
@@ -717,9 +702,6 @@
     <t>Mike Hart Laptop</t>
   </si>
   <si>
-    <t>?? Builder</t>
-  </si>
-  <si>
     <t>ndw1850</t>
   </si>
   <si>
@@ -802,6 +784,18 @@
   </si>
   <si>
     <t>512GB NVMe</t>
+  </si>
+  <si>
+    <t>Store decomission</t>
+  </si>
+  <si>
+    <t>SL7 Builder</t>
+  </si>
+  <si>
+    <t>mantid-mac-pro</t>
+  </si>
+  <si>
+    <t>Mac builds</t>
   </si>
 </sst>
 </file>
@@ -996,7 +990,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1039,7 +1033,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1082,7 +1076,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1125,7 +1119,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1168,7 +1162,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1211,7 +1205,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1254,7 +1248,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1302,7 +1296,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1350,7 +1344,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1398,7 +1392,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1454,7 +1448,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1502,7 +1496,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1550,7 +1544,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1598,12 +1592,60 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="8867775"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1931,7 +1973,7 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1982,7 +2024,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1999,16 +2041,16 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
@@ -2017,7 +2059,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I3">
         <f>VLOOKUP(E3,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2051,7 +2093,7 @@
         <v>40</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I4">
         <f>VLOOKUP(E4,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2064,7 +2106,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -2098,7 +2140,7 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -2132,7 +2174,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -2197,7 +2239,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
@@ -2215,10 +2257,10 @@
         <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I9">
         <f>VLOOKUP(E9,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2265,7 +2307,7 @@
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>61</v>
@@ -2333,10 +2375,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -2351,7 +2393,7 @@
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
@@ -2367,25 +2409,25 @@
     </row>
     <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -2401,25 +2443,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H15" t="s">
         <v>29</v>
@@ -2435,10 +2477,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -2447,16 +2489,16 @@
         <v>25</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I16">
         <f>VLOOKUP(E16,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2469,10 +2511,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -2481,16 +2523,16 @@
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F17" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I17">
         <f>VLOOKUP(E17,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2503,10 +2545,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -2515,16 +2557,16 @@
         <v>25</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F18" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I18">
         <f>VLOOKUP(E18,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2540,25 +2582,25 @@
         <v>63</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F19" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I19">
         <f>VLOOKUP(E19,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2571,28 +2613,28 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
         <v>27</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I20">
         <f>VLOOKUP(E20,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2608,25 +2650,25 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F21" t="s">
         <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I21">
         <f>VLOOKUP(E21,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2639,28 +2681,28 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I22">
         <f>VLOOKUP(E22,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2673,28 +2715,28 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="I23">
         <f>VLOOKUP(E23,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2707,28 +2749,28 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H24" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I24">
         <f>VLOOKUP(E24,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2739,33 +2781,33 @@
         <v>1031</v>
       </c>
       <c r="K24" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H25" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I25">
         <f>VLOOKUP(E25,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2776,7 +2818,7 @@
         <v>1031</v>
       </c>
       <c r="K25" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -2814,10 +2856,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G29" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I29" t="e">
         <f>VLOOKUP(Laptops!E14,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2969,7 +3011,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3011,7 +3053,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -3042,25 +3084,25 @@
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I5">
         <f>VLOOKUP(E5,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3076,25 +3118,25 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
         <v>74</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>76</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>77</v>
-      </c>
-      <c r="H6" t="s">
-        <v>78</v>
       </c>
       <c r="I6">
         <f>VLOOKUP(E6,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3107,7 +3149,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -3141,19 +3183,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
@@ -3162,7 +3204,7 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I8">
         <f>VLOOKUP(E8,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3175,19 +3217,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F9" t="s">
         <v>30</v>
@@ -3196,7 +3238,7 @@
         <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I9">
         <f>VLOOKUP(E9,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3209,28 +3251,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I10">
         <f>VLOOKUP(E10,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3243,25 +3285,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H11" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I11">
         <f>VLOOKUP(E11,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3357,10 +3399,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3376,7 +3418,7 @@
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3408,205 +3450,205 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="I3">
         <f>VLOOKUP(E3,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>405</v>
+        <v>8014</v>
       </c>
       <c r="J3">
         <f>VLOOKUP(H3,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="I4">
         <f>VLOOKUP(E4,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>8014</v>
+        <v>4736</v>
       </c>
       <c r="J4">
         <f>VLOOKUP(H4,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>324</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" t="s">
-        <v>109</v>
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="I5">
         <f>VLOOKUP(E5,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>4736</v>
+        <v>9447</v>
       </c>
       <c r="J5">
         <f>VLOOKUP(H5,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>132</v>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" t="s">
+        <v>85</v>
       </c>
       <c r="I6">
         <f>VLOOKUP(E6,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>9447</v>
+        <v>6345</v>
       </c>
       <c r="J6">
         <f>VLOOKUP(H6,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>658</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" t="s">
-        <v>86</v>
+      <c r="D7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="I7">
         <f>VLOOKUP(E7,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>6345</v>
+        <v>9447</v>
       </c>
       <c r="J7">
         <f>VLOOKUP(H7,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I8">
         <f>VLOOKUP(E8,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3617,231 +3659,234 @@
         <v>658</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>132</v>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
       </c>
       <c r="I9">
         <f>VLOOKUP(E9,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>9447</v>
+        <v>21216</v>
       </c>
       <c r="J9">
         <f>VLOOKUP(H9,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>658</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
+        <v>166</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" t="s">
         <v>91</v>
       </c>
-      <c r="F10" t="s">
-        <v>92</v>
-      </c>
       <c r="G10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" t="s">
-        <v>94</v>
+        <v>131</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="I10">
         <f>VLOOKUP(E10,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>21216</v>
+        <v>24596</v>
       </c>
       <c r="J10">
         <f>VLOOKUP(H10,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>170</v>
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
       <c r="E11" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>137</v>
+        <v>96</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
       </c>
       <c r="I11">
         <f>VLOOKUP(E11,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>24596</v>
+        <v>9045</v>
       </c>
       <c r="J11">
         <f>VLOOKUP(H11,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>2316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>127</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="G12" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="I12">
         <f>VLOOKUP(E12,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>9045</v>
+        <v>16874</v>
       </c>
       <c r="J12">
         <f>VLOOKUP(H12,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>457</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="3">
+        <f>VLOOKUP(E13,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <v>2877</v>
+      </c>
+      <c r="J13" s="3">
+        <f>VLOOKUP(H13,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>1070</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13">
-        <f>VLOOKUP(E13,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>16874</v>
-      </c>
-      <c r="J13">
-        <f>VLOOKUP(H13,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="D14" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14">
         <f>VLOOKUP(E14,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>2877</v>
-      </c>
-      <c r="J14" s="3">
+        <v>10807</v>
+      </c>
+      <c r="J14">
         <f>VLOOKUP(H14,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="I15">
         <f>VLOOKUP(E15,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3852,43 +3897,31 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>205</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" t="s">
+        <v>228</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="I16">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" t="e">
         <f>VLOOKUP(E16,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>10807</v>
-      </c>
-      <c r="J16">
+        <v>#N/A</v>
+      </c>
+      <c r="J16" t="e">
         <f>VLOOKUP(H16,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I17" t="e">
-        <f>VLOOKUP(E17,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <f>VLOOKUP(E34,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J17" t="e">
@@ -3896,16 +3929,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>27</v>
-      </c>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I18" t="e">
         <f>VLOOKUP(E18,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
@@ -3915,7 +3939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I19" t="e">
         <f>VLOOKUP(E19,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
@@ -3925,14 +3949,15 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I20" t="e">
-        <f>VLOOKUP(E20,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J20" t="e">
-        <f>VLOOKUP(H20,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>#N/A</v>
+    <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3986,23 +4011,23 @@
   <sheetData>
     <row r="1" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -4021,29 +4046,29 @@
     </row>
     <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B2">
         <v>405</v>
       </c>
       <c r="C2">
         <f>COUNTIF(Desktops!$E:$E,Benchmarks!$A2) + COUNTIF(Laptops!$E:$E,Benchmarks!$A2) + COUNTIF(Servers!$E:$E,Benchmarks!$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2">
         <v>11</v>
       </c>
       <c r="G2">
         <f>COUNTIF(Desktops!$H:$H,Benchmarks!$E2) + COUNTIF(Laptops!$H:$H,Benchmarks!$E2) + COUNTIF(Servers!$H:$H,Benchmarks!$E2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>1755</v>
@@ -4053,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F3">
         <v>33</v>
@@ -4087,7 +4112,7 @@
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>2877</v>
@@ -4097,7 +4122,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -4109,7 +4134,7 @@
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>3062</v>
@@ -4119,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F6">
         <v>102</v>
@@ -4153,7 +4178,7 @@
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8">
         <v>4736</v>
@@ -4163,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F8">
         <v>427</v>
@@ -4175,7 +4200,7 @@
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B9">
         <v>5397</v>
@@ -4241,7 +4266,7 @@
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12">
         <v>6345</v>
@@ -4251,7 +4276,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F12">
         <v>576</v>
@@ -4273,7 +4298,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F13">
         <v>658</v>
@@ -4285,7 +4310,7 @@
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B14" s="11">
         <v>8141</v>
@@ -4307,7 +4332,7 @@
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B15">
         <v>8657</v>
@@ -4329,7 +4354,7 @@
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B16">
         <v>8765</v>
@@ -4339,7 +4364,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F16">
         <v>991</v>
@@ -4351,7 +4376,7 @@
     </row>
     <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17">
         <v>9045</v>
@@ -4361,7 +4386,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F17">
         <v>1007</v>
@@ -4383,7 +4408,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F18">
         <v>1070</v>
@@ -4395,7 +4420,7 @@
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B19">
         <v>9447</v>
@@ -4405,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F19">
         <v>1097</v>
@@ -4417,7 +4442,7 @@
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B20">
         <v>9995</v>
@@ -4427,7 +4452,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F20">
         <v>1166</v>
@@ -4439,7 +4464,7 @@
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B21">
         <v>10039</v>
@@ -4449,7 +4474,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F21" s="4">
         <v>1198</v>
@@ -4483,7 +4508,7 @@
     </row>
     <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B23" s="11">
         <v>10807</v>
@@ -4493,7 +4518,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23">
         <v>1299</v>
@@ -4505,7 +4530,7 @@
     </row>
     <row r="24" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B24">
         <v>10808</v>
@@ -4515,7 +4540,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F24">
         <v>1409</v>
@@ -4527,7 +4552,7 @@
     </row>
     <row r="25" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B25" s="12">
         <v>16874</v>
@@ -4537,7 +4562,7 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F25">
         <v>1682</v>
@@ -4549,7 +4574,7 @@
     </row>
     <row r="26" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B26" s="14">
         <v>18083</v>
@@ -4559,7 +4584,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F26" s="11">
         <v>2064</v>
@@ -4571,7 +4596,7 @@
     </row>
     <row r="27" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="13">
         <v>21216</v>
@@ -4581,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F27" s="12">
         <v>2316</v>
@@ -4593,7 +4618,7 @@
     </row>
     <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B28" s="13">
         <v>24596</v>
@@ -4603,7 +4628,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F28" s="13">
         <v>3060</v>
@@ -4619,7 +4644,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F29">
         <v>13733</v>
@@ -4635,7 +4660,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F30">
         <v>1031</v>

</xml_diff>

<commit_message>
Updated the hardware list
</commit_message>
<xml_diff>
--- a/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
+++ b/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="236">
   <si>
     <t>Usage</t>
   </si>
@@ -252,9 +252,6 @@
     <t>NVIDIA Quadro NVS 450</t>
   </si>
   <si>
-    <t>Martyn Gigg Desktop</t>
-  </si>
-  <si>
     <t>ndw1213</t>
   </si>
   <si>
@@ -378,21 +375,9 @@
     <t>256GB SSD</t>
   </si>
   <si>
-    <t>Sasview builder</t>
-  </si>
-  <si>
-    <t>mantids-imac</t>
-  </si>
-  <si>
-    <t>iMac</t>
-  </si>
-  <si>
     <t>i3-550 @ 3.2GHz (1 core + HT)</t>
   </si>
   <si>
-    <t>1TB 7200rpm IDE</t>
-  </si>
-  <si>
     <t>ATI Radeon HD5670</t>
   </si>
   <si>
@@ -705,9 +690,6 @@
     <t>512GB NVMe</t>
   </si>
   <si>
-    <t>Store decomission</t>
-  </si>
-  <si>
     <t>SL7 Builder</t>
   </si>
   <si>
@@ -717,9 +699,6 @@
     <t>Mac builds</t>
   </si>
   <si>
-    <t>Sam Jones</t>
-  </si>
-  <si>
     <t>ndw1597</t>
   </si>
   <si>
@@ -811,6 +790,30 @@
   </si>
   <si>
     <t>Intel HD Graphics 530</t>
+  </si>
+  <si>
+    <t>Anthony Lim Desktop</t>
+  </si>
+  <si>
+    <t>Martyn Gigg (SX) desktop</t>
+  </si>
+  <si>
+    <t>ndw2185</t>
+  </si>
+  <si>
+    <t>Precision 5820</t>
+  </si>
+  <si>
+    <t>i9-7960X@2.8GHz</t>
+  </si>
+  <si>
+    <t>nVidia RTX4000</t>
+  </si>
+  <si>
+    <t>i9-9900@3.1GHZ</t>
+  </si>
+  <si>
+    <t>Harry Saunders</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1055,7 +1058,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1098,7 +1101,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1141,7 +1144,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1184,7 +1187,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1227,7 +1230,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1270,7 +1273,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1318,7 +1321,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1366,7 +1369,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1414,7 +1417,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1470,7 +1473,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1518,7 +1521,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1566,7 +1569,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1614,7 +1617,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1662,7 +1665,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1710,7 +1713,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1758,7 +1761,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1806,7 +1809,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1854,7 +1857,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1902,7 +1905,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1950,7 +1953,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1998,7 +2001,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2046,7 +2049,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2060,6 +2063,102 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="9525000" cy="9058275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9058275"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="8839200"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2377,10 +2476,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2430,7 +2529,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2444,10 +2543,10 @@
     </row>
     <row r="3" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -2465,7 +2564,7 @@
         <v>38</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I3">
         <f>VLOOKUP(E3,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2478,19 +2577,19 @@
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
@@ -2499,7 +2598,7 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4">
         <f>VLOOKUP(E4,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2512,19 +2611,19 @@
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
@@ -2533,7 +2632,7 @@
         <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5">
         <f>VLOOKUP(E5,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2546,28 +2645,28 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6">
         <f>VLOOKUP(E6,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2580,7 +2679,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -2598,10 +2697,10 @@
         <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I7">
         <f>VLOOKUP(E7,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2648,10 +2747,10 @@
     </row>
     <row r="9" spans="1:10" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
@@ -2666,7 +2765,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>29</v>
@@ -2682,16 +2781,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -2700,7 +2799,7 @@
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
         <v>29</v>
@@ -2716,33 +2815,33 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
         <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -2758,25 +2857,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
@@ -2792,10 +2891,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -2804,16 +2903,16 @@
         <v>25</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I14">
         <f>VLOOKUP(E14,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2826,10 +2925,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -2838,16 +2937,16 @@
         <v>25</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I15">
         <f>VLOOKUP(E15,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2860,10 +2959,10 @@
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -2872,16 +2971,16 @@
         <v>25</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I16">
         <f>VLOOKUP(E16,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2894,28 +2993,28 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="I17">
         <f>VLOOKUP(E17,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2928,28 +3027,28 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F18" t="s">
         <v>27</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I18">
         <f>VLOOKUP(E18,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2962,28 +3061,28 @@
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B19" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I19">
         <f>VLOOKUP(E19,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -2996,28 +3095,28 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="I20">
         <f>VLOOKUP(E20,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3030,28 +3129,28 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F21" t="s">
         <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H21" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I21">
         <f>VLOOKUP(E21,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3064,28 +3163,28 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
       </c>
       <c r="G22" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H22" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I22">
         <f>VLOOKUP(E22,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3098,28 +3197,28 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I23">
         <f>VLOOKUP(E23,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3132,28 +3231,28 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I24">
         <f>VLOOKUP(E24,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3166,28 +3265,28 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I25">
         <f>VLOOKUP(E25,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3200,28 +3299,28 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="I26">
         <f>VLOOKUP(E26,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3233,34 +3332,58 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="G27" s="2" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I27" t="e">
+        <v>233</v>
+      </c>
+      <c r="I27">
+        <f>VLOOKUP(E27,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <v>26030</v>
+      </c>
+      <c r="J27">
+        <f>VLOOKUP(H27,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>13266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I28" t="e">
         <f>VLOOKUP(Laptops!E14,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J27">
-        <f>VLOOKUP(H27,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+      <c r="J28">
+        <f>VLOOKUP(H28,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>427</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I28" t="e">
-        <f>VLOOKUP(Laptops!E15,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J28" t="e">
-        <f>VLOOKUP(H28,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I29" t="e">
-        <f>VLOOKUP(Laptops!E16,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <f>VLOOKUP(Laptops!E15,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J29" t="e">
@@ -3270,7 +3393,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I30" t="e">
-        <f>VLOOKUP(E30,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <f>VLOOKUP(Laptops!E16,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J30" t="e">
@@ -3278,9 +3401,19 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I31" t="e">
+        <f>VLOOKUP(E31,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J31" t="e">
+        <f>VLOOKUP(H31,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="I1:I35 I37:I1048576">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3292,7 +3425,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3365,7 +3546,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3407,7 +3588,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -3438,25 +3619,25 @@
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I5">
         <f>VLOOKUP(E5,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3469,28 +3650,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>67</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>68</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>69</v>
-      </c>
-      <c r="H6" t="s">
-        <v>70</v>
       </c>
       <c r="I6">
         <f>VLOOKUP(E6,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3503,7 +3684,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -3537,19 +3718,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F8" t="s">
         <v>30</v>
@@ -3558,7 +3739,7 @@
         <v>21</v>
       </c>
       <c r="H8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I8">
         <f>VLOOKUP(E8,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3571,19 +3752,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
         <v>30</v>
@@ -3592,7 +3773,7 @@
         <v>21</v>
       </c>
       <c r="H9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I9">
         <f>VLOOKUP(E9,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3605,28 +3786,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I10">
         <f>VLOOKUP(E10,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3639,25 +3820,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H11" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I11">
         <f>VLOOKUP(E11,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3753,10 +3934,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A14" sqref="A13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3772,7 +3953,7 @@
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3804,35 +3985,35 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
         <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I3">
         <f>VLOOKUP(E3,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3843,30 +4024,30 @@
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I4">
         <f>VLOOKUP(E4,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3877,21 +4058,21 @@
         <v>1682</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>27</v>
@@ -3900,7 +4081,7 @@
         <v>33</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I5">
         <f>VLOOKUP(E5,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3911,30 +4092,30 @@
         <v>658</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
         <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
         <v>74</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>76</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>77</v>
-      </c>
-      <c r="H6" t="s">
-        <v>78</v>
       </c>
       <c r="I6">
         <f>VLOOKUP(E6,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3945,30 +4126,30 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I7">
         <f>VLOOKUP(E7,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -3979,30 +4160,30 @@
         <v>658</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I8">
         <f>VLOOKUP(E8,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -4013,30 +4194,30 @@
         <v>658</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" t="s">
         <v>82</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>83</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>84</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>85</v>
-      </c>
-      <c r="H9" t="s">
-        <v>86</v>
       </c>
       <c r="I9">
         <f>VLOOKUP(E9,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -4047,30 +4228,30 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I10">
         <f>VLOOKUP(E10,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -4081,24 +4262,24 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
         <v>88</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" t="s">
-        <v>89</v>
       </c>
       <c r="H11" t="s">
         <v>34</v>
@@ -4112,30 +4293,30 @@
         <v>457</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I12">
         <f>VLOOKUP(E12,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -4146,67 +4327,64 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I13" s="3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13">
         <f>VLOOKUP(E13,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>2877</v>
-      </c>
-      <c r="J13" s="3">
+        <v>10807</v>
+      </c>
+      <c r="J13">
         <f>VLOOKUP(H13,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1070</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I14">
         <f>VLOOKUP(E14,Benchmarks!$A$2:$B$942,2,FALSE)</f>
@@ -4217,55 +4395,31 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>180</v>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" t="s">
+        <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I15">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" t="e">
         <f>VLOOKUP(E15,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>10807</v>
-      </c>
-      <c r="J15">
+        <v>#N/A</v>
+      </c>
+      <c r="J15" t="e">
         <f>VLOOKUP(H15,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>202</v>
-      </c>
-      <c r="B16" t="s">
-        <v>201</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
-      </c>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I16" t="e">
-        <f>VLOOKUP(E16,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <f>VLOOKUP(E33,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J16" t="e">
@@ -4275,7 +4429,7 @@
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I17" t="e">
-        <f>VLOOKUP(E34,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <f>VLOOKUP(E17,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J17" t="e">
@@ -4293,24 +4447,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I19" t="e">
-        <f>VLOOKUP(E19,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J19" t="e">
-        <f>VLOOKUP(H19,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="2" t="s">
+    <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4354,7 +4498,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4365,23 +4509,23 @@
   <sheetData>
     <row r="1" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -4400,7 +4544,7 @@
     </row>
     <row r="2" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B2">
         <v>405</v>
@@ -4410,7 +4554,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F2">
         <v>11</v>
@@ -4422,7 +4566,7 @@
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>1755</v>
@@ -4432,7 +4576,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F3">
         <v>33</v>
@@ -4466,17 +4610,17 @@
     </row>
     <row r="5" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B5">
         <v>2877</v>
       </c>
       <c r="C5">
         <f>COUNTIF(Desktops!$E:$E,Benchmarks!$A5) + COUNTIF(Laptops!$E:$E,Benchmarks!$A5) + COUNTIF(Servers!$E:$E,Benchmarks!$A5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -4488,7 +4632,7 @@
     </row>
     <row r="6" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>3062</v>
@@ -4498,7 +4642,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F6">
         <v>102</v>
@@ -4520,7 +4664,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7">
         <v>324</v>
@@ -4532,7 +4676,7 @@
     </row>
     <row r="8" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B8">
         <v>4736</v>
@@ -4542,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F8">
         <v>427</v>
@@ -4554,7 +4698,7 @@
     </row>
     <row r="9" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <v>5397</v>
@@ -4576,7 +4720,7 @@
     </row>
     <row r="10" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>5478</v>
@@ -4620,7 +4764,7 @@
     </row>
     <row r="12" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12">
         <v>6345</v>
@@ -4630,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F12">
         <v>576</v>
@@ -4642,7 +4786,7 @@
     </row>
     <row r="13" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>8014</v>
@@ -4652,7 +4796,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F13">
         <v>658</v>
@@ -4664,7 +4808,7 @@
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B14" s="11">
         <v>8141</v>
@@ -4674,7 +4818,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <v>684</v>
@@ -4686,7 +4830,7 @@
     </row>
     <row r="15" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B15">
         <v>8657</v>
@@ -4708,7 +4852,7 @@
     </row>
     <row r="16" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B16">
         <v>8765</v>
@@ -4718,7 +4862,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F16">
         <v>991</v>
@@ -4730,7 +4874,7 @@
     </row>
     <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17">
         <v>9045</v>
@@ -4740,7 +4884,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F17">
         <v>1007</v>
@@ -4762,7 +4906,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F18">
         <v>1031</v>
@@ -4774,7 +4918,7 @@
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B19">
         <v>9447</v>
@@ -4784,7 +4928,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F19">
         <v>1070</v>
@@ -4796,7 +4940,7 @@
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B20">
         <v>9995</v>
@@ -4806,19 +4950,19 @@
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20">
         <v>1097</v>
       </c>
       <c r="G20">
         <f>COUNTIF(Desktops!$H:$H,Benchmarks!$E19) + COUNTIF(Laptops!$H:$H,Benchmarks!$E19) + COUNTIF(Servers!$H:$H,Benchmarks!$E19)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B21">
         <v>10039</v>
@@ -4828,7 +4972,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F21" s="4">
         <v>1122</v>
@@ -4850,7 +4994,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F22" s="4">
         <v>1215</v>
@@ -4862,7 +5006,7 @@
     </row>
     <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B23" s="11">
         <v>10807</v>
@@ -4884,7 +5028,7 @@
     </row>
     <row r="24" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B24">
         <v>10808</v>
@@ -4894,7 +5038,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F24">
         <v>1299</v>
@@ -4906,7 +5050,7 @@
     </row>
     <row r="25" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B25" s="12">
         <v>16874</v>
@@ -4916,7 +5060,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F25">
         <v>1409</v>
@@ -4928,7 +5072,7 @@
     </row>
     <row r="26" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B26" s="14">
         <v>18083</v>
@@ -4938,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F26">
         <v>1682</v>
@@ -4950,7 +5094,7 @@
     </row>
     <row r="27" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="13">
         <v>21216</v>
@@ -4960,7 +5104,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F27" s="16">
         <v>2064</v>
@@ -4972,7 +5116,7 @@
     </row>
     <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B28" s="13">
         <v>24596</v>
@@ -4982,7 +5126,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F28" s="13">
         <v>2316</v>
@@ -4994,7 +5138,7 @@
     </row>
     <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B29">
         <v>15130</v>
@@ -5004,7 +5148,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F29" s="13">
         <v>3060</v>
@@ -5015,12 +5159,18 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30">
+        <v>26030</v>
+      </c>
       <c r="C30">
         <f>COUNTIF(Desktops!$E:$E,Benchmarks!$A30) + COUNTIF(Laptops!$E:$E,Benchmarks!$A30) + COUNTIF(Servers!$E:$E,Benchmarks!$A30)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F30">
         <v>13733</v>
@@ -5031,9 +5181,25 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B31">
+        <v>18619</v>
+      </c>
       <c r="C31">
         <f>COUNTIF(Desktops!$E:$E,Benchmarks!$A31) + COUNTIF(Laptops!$E:$E,Benchmarks!$A31) + COUNTIF(Servers!$E:$E,Benchmarks!$A31)</f>
         <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F31">
+        <v>13266</v>
+      </c>
+      <c r="G31">
+        <f>COUNTIF(Desktops!$H:$H,Benchmarks!$E30) + COUNTIF(Laptops!$H:$H,Benchmarks!$E30) + COUNTIF(Servers!$H:$H,Benchmarks!$E30)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5078,7 +5244,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32:G1048576 G1:G30">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
@@ -5116,7 +5282,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B31">
+  <conditionalFormatting sqref="B2:B999">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -5128,7 +5294,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
+  <conditionalFormatting sqref="F2:F999">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5170,7 +5336,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G32:G1048576 G1:G30</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
hardware update and IMSSC progress report
</commit_message>
<xml_diff>
--- a/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
+++ b/Project-Management/Hardware/RAL/Mantid Hardware.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="525" yWindow="555" windowWidth="21495" windowHeight="13725"/>
+    <workbookView xWindow="525" yWindow="555" windowWidth="14805" windowHeight="1800"/>
   </bookViews>
   <sheets>
     <sheet name="Desktops" sheetId="4" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="236">
   <si>
     <t>Usage</t>
   </si>
@@ -786,17 +786,41 @@
     <t>New suggested PC spec</t>
   </si>
   <si>
-    <t>Optiplex 7070</t>
-  </si>
-  <si>
     <t>Imaging PC  Loan - from Tino</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Mac 1</t>
+  </si>
+  <si>
+    <t>Mac 2</t>
+  </si>
+  <si>
+    <t>old mac to Build server</t>
+  </si>
+  <si>
+    <t>Build server</t>
+  </si>
+  <si>
+    <t>New Pc</t>
+  </si>
+  <si>
+    <t>Old PC</t>
+  </si>
+  <si>
+    <t>Small form factor Precision</t>
+  </si>
+  <si>
+    <t>? Placement or harrys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -867,8 +891,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,8 +928,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -920,14 +957,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -975,9 +1028,13 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2223,6 +2280,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9115425"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2516,10 +2621,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="A11:K11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2535,7 +2640,7 @@
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2566,8 +2671,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>125</v>
       </c>
@@ -2581,7 +2692,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2614,8 +2725,14 @@
         <f>VLOOKUP(H3,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>987</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>214</v>
       </c>
@@ -2648,16 +2765,22 @@
         <f>VLOOKUP(H4,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>987</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>204</v>
       </c>
@@ -2691,8 +2814,8 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>221</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2724,8 +2847,11 @@
         <f>VLOOKUP(H7,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>987</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>160</v>
       </c>
@@ -2758,8 +2884,14 @@
         <f>VLOOKUP(H8,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>1409</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>203</v>
       </c>
@@ -2792,8 +2924,14 @@
         <f>VLOOKUP(H9,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>1409</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>132</v>
       </c>
@@ -2826,8 +2964,14 @@
         <f>VLOOKUP(H10,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>1409</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>206</v>
       </c>
@@ -2860,8 +3004,14 @@
         <f>VLOOKUP(H11,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>1007</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>227</v>
+      </c>
+      <c r="L11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>199</v>
       </c>
@@ -2895,7 +3045,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>198</v>
       </c>
@@ -2929,7 +3079,7 @@
         <v>13733</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>202</v>
       </c>
@@ -2963,8 +3113,8 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>200</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2997,7 +3147,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>201</v>
       </c>
@@ -3031,7 +3181,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>192</v>
       </c>
@@ -3065,7 +3215,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>205</v>
       </c>
@@ -3098,8 +3248,14 @@
         <f>VLOOKUP(H18,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>1122</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>228</v>
+      </c>
+      <c r="L18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>207</v>
       </c>
@@ -3133,7 +3289,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>215</v>
       </c>
@@ -3166,79 +3322,134 @@
         <f>VLOOKUP(H20,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>13266</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G21" s="2" t="s">
+      <c r="K20" t="s">
+        <v>229</v>
+      </c>
+      <c r="L20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="I26">
+        <f>VLOOKUP(E26,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <v>18619</v>
+      </c>
+      <c r="J26">
+        <f>VLOOKUP(H26,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I27" t="e">
+        <f>VLOOKUP(E27,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J27" t="e">
+        <f>VLOOKUP(H27,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I28" t="e">
+        <f>VLOOKUP(E28,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J28" t="e">
+        <f>VLOOKUP(H28,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I21" t="e">
-        <f>VLOOKUP(E21,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+      <c r="I30" t="e">
+        <f>VLOOKUP(E29,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J21">
-        <f>VLOOKUP(H21,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+      <c r="J30">
+        <f>VLOOKUP(H30,Benchmarks!$E$2:$F$947,2,FALSE)</f>
         <v>427</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>225</v>
-      </c>
-      <c r="B22" t="s">
-        <v>191</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F22" t="s">
-        <v>210</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="I22">
-        <f>VLOOKUP(E22,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>18619</v>
-      </c>
-      <c r="J22">
-        <f>VLOOKUP(H22,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I23" t="e">
-        <f>VLOOKUP(E23,Benchmarks!$A$2:$B$942,2,FALSE)</f>
+    <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>150</v>
+      </c>
+      <c r="I31" t="e">
+        <f>VLOOKUP(E30,Benchmarks!$A$2:$B$942,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J23" t="e">
-        <f>VLOOKUP(H23,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I24" t="e">
-        <f>VLOOKUP(E24,Benchmarks!$A$2:$B$942,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J24" t="e">
-        <f>VLOOKUP(H24,Benchmarks!$E$2:$F$947,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="J31">
+        <f>VLOOKUP(H31,Benchmarks!$E$2:$F$947,2,FALSE)</f>
+        <v>3060</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I30:I1048576 I1:I28">
+  <conditionalFormatting sqref="I34:I1048576 I1:I24 I26:I32">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -3250,7 +3461,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="J1:J24 J26:J1048576">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -3262,7 +3473,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I33">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3274,7 +3485,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I33">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3286,7 +3497,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3298,7 +3509,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3763,7 +3974,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5099,7 +5310,7 @@
       </c>
       <c r="G30">
         <f>COUNTIF(Desktops!$H:$H,Benchmarks!$E29) + COUNTIF(Laptops!$H:$H,Benchmarks!$E29) + COUNTIF(Servers!$H:$H,Benchmarks!$E29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>